<commit_message>
Added periodic & upfront related scenarios
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/1109-MS-EPP-DB-SAR-REC-NON-RNI-CTPD-SAR-MD-TR-1-LateRepayment-Makerepayment1.xlsx
+++ b/Mifos Automation Excels/Client/1109-MS-EPP-DB-SAR-REC-NON-RNI-CTPD-SAR-MD-TR-1-LateRepayment-Makerepayment1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="495" windowWidth="15015" windowHeight="7620" tabRatio="439" activeTab="2"/>
+    <workbookView xWindow="180" yWindow="495" windowWidth="15015" windowHeight="7620" tabRatio="439" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="9" r:id="rId1"/>
@@ -127,7 +127,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,12 +152,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -171,12 +165,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -544,10 +537,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -557,7 +550,7 @@
     <col min="5" max="6" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -577,86 +570,83 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
         <v>10000</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>833.33</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6">
-        <v>0</v>
-      </c>
-      <c r="E2" s="7">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6">
         <v>9166.67</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <v>833.33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
         <v>666.67</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>100</v>
       </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6">
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
         <v>566.66999999999996</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
-        <v>0</v>
-      </c>
-      <c r="B4" s="6">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
-        <v>0</v>
-      </c>
-      <c r="B5" s="6">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G7" s="4"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -667,7 +657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -735,543 +725,543 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B2" s="6"/>
-      <c r="C2" s="8">
+      <c r="B2" s="5"/>
+      <c r="C2" s="7">
         <v>42005</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="5">
+      <c r="D2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="4">
         <v>10000</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6">
-        <v>0</v>
-      </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6">
-        <v>0</v>
-      </c>
-      <c r="L2" s="6">
-        <v>0</v>
-      </c>
-      <c r="M2" s="6"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5">
+        <v>0</v>
+      </c>
+      <c r="L2" s="5">
+        <v>0</v>
+      </c>
+      <c r="M2" s="5"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>31</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>42036</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>42050</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="6">
+      <c r="E3" s="8"/>
+      <c r="F3" s="5">
         <v>833.33</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>9166.67</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>100</v>
       </c>
-      <c r="I3" s="6">
-        <v>0</v>
-      </c>
-      <c r="J3" s="6">
-        <v>0</v>
-      </c>
-      <c r="K3" s="6">
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5">
         <v>933.33</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="5">
         <v>933.33</v>
       </c>
-      <c r="M3" s="6">
-        <v>0</v>
-      </c>
-      <c r="N3" s="6">
+      <c r="M3" s="5">
+        <v>0</v>
+      </c>
+      <c r="N3" s="5">
         <v>933.33</v>
       </c>
-      <c r="P3" s="6">
+      <c r="P3" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>28</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>42064</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5">
         <v>833.33</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <v>8333.34</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>100</v>
       </c>
-      <c r="I4" s="6">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6">
-        <v>0</v>
-      </c>
-      <c r="K4" s="6">
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
         <v>933.33</v>
       </c>
-      <c r="L4" s="6">
-        <v>0</v>
-      </c>
-      <c r="M4" s="6">
-        <v>0</v>
-      </c>
-      <c r="N4" s="6">
-        <v>0</v>
-      </c>
-      <c r="P4" s="6">
+      <c r="L4" s="5">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0</v>
+      </c>
+      <c r="N4" s="5">
+        <v>0</v>
+      </c>
+      <c r="P4" s="5">
         <v>933.33</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>31</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>42095</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5">
         <v>833.33</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <v>7500.01</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>91.67</v>
       </c>
-      <c r="I5" s="6">
-        <v>0</v>
-      </c>
-      <c r="J5" s="6">
-        <v>0</v>
-      </c>
-      <c r="K5" s="6">
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="5">
         <v>925</v>
       </c>
-      <c r="L5" s="6">
-        <v>0</v>
-      </c>
-      <c r="M5" s="6">
-        <v>0</v>
-      </c>
-      <c r="N5" s="6">
-        <v>0</v>
-      </c>
-      <c r="P5" s="6">
+      <c r="L5" s="5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="5">
+        <v>0</v>
+      </c>
+      <c r="P5" s="5">
         <v>925</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>30</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>42125</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5">
         <v>833.33</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <v>6666.68</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <v>75</v>
       </c>
-      <c r="I6" s="6">
-        <v>0</v>
-      </c>
-      <c r="J6" s="6">
-        <v>0</v>
-      </c>
-      <c r="K6" s="6">
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0</v>
+      </c>
+      <c r="K6" s="5">
         <v>908.33</v>
       </c>
-      <c r="L6" s="6">
-        <v>0</v>
-      </c>
-      <c r="M6" s="6">
-        <v>0</v>
-      </c>
-      <c r="N6" s="6">
-        <v>0</v>
-      </c>
-      <c r="P6" s="6">
+      <c r="L6" s="5">
+        <v>0</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0</v>
+      </c>
+      <c r="N6" s="5">
+        <v>0</v>
+      </c>
+      <c r="P6" s="5">
         <v>908.33</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>31</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>42156</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5">
         <v>833.33</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>5833.35</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <v>66.67</v>
       </c>
-      <c r="I7" s="6">
-        <v>0</v>
-      </c>
-      <c r="J7" s="6">
-        <v>0</v>
-      </c>
-      <c r="K7" s="6">
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0</v>
+      </c>
+      <c r="K7" s="5">
         <v>900</v>
       </c>
-      <c r="L7" s="6">
-        <v>0</v>
-      </c>
-      <c r="M7" s="6">
-        <v>0</v>
-      </c>
-      <c r="N7" s="6">
-        <v>0</v>
-      </c>
-      <c r="P7" s="6">
+      <c r="L7" s="5">
+        <v>0</v>
+      </c>
+      <c r="M7" s="5">
+        <v>0</v>
+      </c>
+      <c r="N7" s="5">
+        <v>0</v>
+      </c>
+      <c r="P7" s="5">
         <v>900</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>30</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>42186</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5">
         <v>833.33</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <v>5000.0200000000004</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <v>58.33</v>
       </c>
-      <c r="I8" s="6">
-        <v>0</v>
-      </c>
-      <c r="J8" s="6">
-        <v>0</v>
-      </c>
-      <c r="K8" s="6">
+      <c r="I8" s="5">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0</v>
+      </c>
+      <c r="K8" s="5">
         <v>891.66</v>
       </c>
-      <c r="L8" s="6">
-        <v>0</v>
-      </c>
-      <c r="M8" s="6">
-        <v>0</v>
-      </c>
-      <c r="N8" s="6">
-        <v>0</v>
-      </c>
-      <c r="P8" s="6">
+      <c r="L8" s="5">
+        <v>0</v>
+      </c>
+      <c r="M8" s="5">
+        <v>0</v>
+      </c>
+      <c r="N8" s="5">
+        <v>0</v>
+      </c>
+      <c r="P8" s="5">
         <v>891.66</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>31</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <v>42217</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5">
         <v>833.33</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>4166.6899999999996</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <v>50</v>
       </c>
-      <c r="I9" s="6">
-        <v>0</v>
-      </c>
-      <c r="J9" s="6">
-        <v>0</v>
-      </c>
-      <c r="K9" s="6">
+      <c r="I9" s="5">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5">
+        <v>0</v>
+      </c>
+      <c r="K9" s="5">
         <v>883.33</v>
       </c>
-      <c r="L9" s="6">
-        <v>0</v>
-      </c>
-      <c r="M9" s="6">
-        <v>0</v>
-      </c>
-      <c r="N9" s="6">
-        <v>0</v>
-      </c>
-      <c r="P9" s="6">
+      <c r="L9" s="5">
+        <v>0</v>
+      </c>
+      <c r="M9" s="5">
+        <v>0</v>
+      </c>
+      <c r="N9" s="5">
+        <v>0</v>
+      </c>
+      <c r="P9" s="5">
         <v>883.33</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>31</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <v>42248</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6">
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5">
         <v>833.33</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <v>3333.36</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <v>41.67</v>
       </c>
-      <c r="I10" s="6">
-        <v>0</v>
-      </c>
-      <c r="J10" s="6">
-        <v>0</v>
-      </c>
-      <c r="K10" s="6">
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5">
+        <v>0</v>
+      </c>
+      <c r="K10" s="5">
         <v>875</v>
       </c>
-      <c r="L10" s="6">
-        <v>0</v>
-      </c>
-      <c r="M10" s="6">
-        <v>0</v>
-      </c>
-      <c r="N10" s="6">
-        <v>0</v>
-      </c>
-      <c r="P10" s="6">
+      <c r="L10" s="5">
+        <v>0</v>
+      </c>
+      <c r="M10" s="5">
+        <v>0</v>
+      </c>
+      <c r="N10" s="5">
+        <v>0</v>
+      </c>
+      <c r="P10" s="5">
         <v>875</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>9</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>30</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="7">
         <v>42278</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5">
         <v>833.33</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <v>2500.0300000000002</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <v>33.33</v>
       </c>
-      <c r="I11" s="6">
-        <v>0</v>
-      </c>
-      <c r="J11" s="6">
-        <v>0</v>
-      </c>
-      <c r="K11" s="6">
+      <c r="I11" s="5">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5">
+        <v>0</v>
+      </c>
+      <c r="K11" s="5">
         <v>866.66</v>
       </c>
-      <c r="L11" s="6">
-        <v>0</v>
-      </c>
-      <c r="M11" s="6">
-        <v>0</v>
-      </c>
-      <c r="N11" s="6">
-        <v>0</v>
-      </c>
-      <c r="P11" s="6">
+      <c r="L11" s="5">
+        <v>0</v>
+      </c>
+      <c r="M11" s="5">
+        <v>0</v>
+      </c>
+      <c r="N11" s="5">
+        <v>0</v>
+      </c>
+      <c r="P11" s="5">
         <v>866.66</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
+      <c r="A12" s="5">
         <v>10</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>31</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>42309</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5">
         <v>833.33</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="6">
         <v>1666.7</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="5">
         <v>25</v>
       </c>
-      <c r="I12" s="6">
-        <v>0</v>
-      </c>
-      <c r="J12" s="6">
-        <v>0</v>
-      </c>
-      <c r="K12" s="6">
+      <c r="I12" s="5">
+        <v>0</v>
+      </c>
+      <c r="J12" s="5">
+        <v>0</v>
+      </c>
+      <c r="K12" s="5">
         <v>858.33</v>
       </c>
-      <c r="L12" s="6">
-        <v>0</v>
-      </c>
-      <c r="M12" s="6">
-        <v>0</v>
-      </c>
-      <c r="N12" s="6">
-        <v>0</v>
-      </c>
-      <c r="P12" s="6">
+      <c r="L12" s="5">
+        <v>0</v>
+      </c>
+      <c r="M12" s="5">
+        <v>0</v>
+      </c>
+      <c r="N12" s="5">
+        <v>0</v>
+      </c>
+      <c r="P12" s="5">
         <v>858.33</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>11</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>30</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>42339</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6">
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5">
         <v>833.33</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="5">
         <v>833.37</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="5">
         <v>16.670000000000002</v>
       </c>
-      <c r="I13" s="6">
-        <v>0</v>
-      </c>
-      <c r="J13" s="6">
-        <v>0</v>
-      </c>
-      <c r="K13" s="6">
+      <c r="I13" s="5">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5">
+        <v>0</v>
+      </c>
+      <c r="K13" s="5">
         <v>850</v>
       </c>
-      <c r="L13" s="6">
-        <v>0</v>
-      </c>
-      <c r="M13" s="6">
-        <v>0</v>
-      </c>
-      <c r="N13" s="6">
-        <v>0</v>
-      </c>
-      <c r="P13" s="6">
+      <c r="L13" s="5">
+        <v>0</v>
+      </c>
+      <c r="M13" s="5">
+        <v>0</v>
+      </c>
+      <c r="N13" s="5">
+        <v>0</v>
+      </c>
+      <c r="P13" s="5">
         <v>850</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
+      <c r="A14" s="5">
         <v>12</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>31</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <v>42370</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6">
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5">
         <v>833.37</v>
       </c>
-      <c r="G14" s="6">
-        <v>0</v>
-      </c>
-      <c r="H14" s="6">
+      <c r="G14" s="5">
+        <v>0</v>
+      </c>
+      <c r="H14" s="5">
         <v>8.33</v>
       </c>
-      <c r="I14" s="6">
-        <v>0</v>
-      </c>
-      <c r="J14" s="6">
-        <v>0</v>
-      </c>
-      <c r="K14" s="6">
+      <c r="I14" s="5">
+        <v>0</v>
+      </c>
+      <c r="J14" s="5">
+        <v>0</v>
+      </c>
+      <c r="K14" s="5">
         <v>841.7</v>
       </c>
-      <c r="L14" s="6">
-        <v>0</v>
-      </c>
-      <c r="M14" s="6">
-        <v>0</v>
-      </c>
-      <c r="N14" s="6">
-        <v>0</v>
-      </c>
-      <c r="P14" s="6">
+      <c r="L14" s="5">
+        <v>0</v>
+      </c>
+      <c r="M14" s="5">
+        <v>0</v>
+      </c>
+      <c r="N14" s="5">
+        <v>0</v>
+      </c>
+      <c r="P14" s="5">
         <v>841.7</v>
       </c>
     </row>
@@ -1302,98 +1292,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="11">
+      <c r="A2" s="10">
         <v>2622</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="12">
         <v>42050</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="10">
         <v>933.33</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="10">
         <v>833.33</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="10">
         <v>100</v>
       </c>
-      <c r="H2" s="11">
-        <v>0</v>
-      </c>
-      <c r="I2" s="11">
-        <v>0</v>
-      </c>
-      <c r="J2" s="14">
+      <c r="H2" s="10">
+        <v>0</v>
+      </c>
+      <c r="I2" s="10">
+        <v>0</v>
+      </c>
+      <c r="J2" s="13">
         <v>9166.67</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="11">
+      <c r="A3" s="10">
         <v>2621</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="12">
         <v>42005</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="14">
         <v>10000</v>
       </c>
-      <c r="F3" s="11">
-        <v>0</v>
-      </c>
-      <c r="G3" s="11">
-        <v>0</v>
-      </c>
-      <c r="H3" s="11">
-        <v>0</v>
-      </c>
-      <c r="I3" s="11">
-        <v>0</v>
-      </c>
-      <c r="J3" s="15">
+      <c r="F3" s="10">
+        <v>0</v>
+      </c>
+      <c r="G3" s="10">
+        <v>0</v>
+      </c>
+      <c r="H3" s="10">
+        <v>0</v>
+      </c>
+      <c r="I3" s="10">
+        <v>0</v>
+      </c>
+      <c r="J3" s="14">
         <v>10000</v>
       </c>
     </row>

</xml_diff>